<commit_message>
more data from May Prince Island trip
</commit_message>
<xml_diff>
--- a/Prince Island/COMU photos/PI_COMU_counts.xlsx
+++ b/Prince Island/COMU photos/PI_COMU_counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekelsey\Documents\FieldWork\Channel Islands\Prince Island\COMU photos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekelsey\Documents\WERC-SC\Prince Island\COMU photos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>year</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>label photographs: "MMDDYY_COMU_PI_group#_photograph#</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>lower colony on northern promentary of island, 3 more COMU right above colony</t>
+  </si>
+  <si>
+    <t>upper colony on northern promentary of island, 3 more COMU right above colony</t>
   </si>
 </sst>
 </file>
@@ -475,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A10" sqref="A10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,6 +523,9 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
@@ -544,7 +556,7 @@
         <v>73</v>
       </c>
       <c r="I2">
-        <f>AVERAGE(F2:H2)</f>
+        <f t="shared" ref="I2:I11" si="0">AVERAGE(F2:H2)</f>
         <v>73.333333333333329</v>
       </c>
     </row>
@@ -574,7 +586,7 @@
         <v>73</v>
       </c>
       <c r="I3">
-        <f>AVERAGE(F3:H3)</f>
+        <f t="shared" si="0"/>
         <v>72.333333333333329</v>
       </c>
     </row>
@@ -604,7 +616,7 @@
         <v>79</v>
       </c>
       <c r="I4">
-        <f>AVERAGE(F4:H4)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
@@ -634,7 +646,7 @@
         <v>72</v>
       </c>
       <c r="I5">
-        <f>AVERAGE(F5:H5)</f>
+        <f t="shared" si="0"/>
         <v>72.666666666666671</v>
       </c>
     </row>
@@ -664,7 +676,7 @@
         <v>9</v>
       </c>
       <c r="I6">
-        <f>AVERAGE(F6:H6)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -694,7 +706,7 @@
         <v>37</v>
       </c>
       <c r="I7">
-        <f>AVERAGE(F7:H7)</f>
+        <f t="shared" si="0"/>
         <v>36.666666666666664</v>
       </c>
     </row>
@@ -724,8 +736,104 @@
         <v>39</v>
       </c>
       <c r="I8">
-        <f>AVERAGE(F8:H8)</f>
+        <f t="shared" si="0"/>
         <v>39.333333333333336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2018</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>20180514</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>21</v>
+      </c>
+      <c r="G9">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>22</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>22.666666666666668</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>20180514</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>73</v>
+      </c>
+      <c r="G10">
+        <v>75</v>
+      </c>
+      <c r="H10">
+        <v>72</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2018</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>20180514</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>32</v>
+      </c>
+      <c r="H11">
+        <v>33</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>32.333333333333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>